<commit_message>
Two Pointer + Hashing - Day 2
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LEARNING\java-learning\java-program-structured\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1A3978-B4D7-457C-A3D8-40C412004DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8C0303-3612-468A-A948-64DB83E758CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{DA8D99D3-37C9-4A5B-806F-CEB05F07CB82}"/>
   </bookViews>
@@ -385,12 +385,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,10 +787,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91DCB90B-2EC4-4C76-AAEF-2887C0F06756}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A9" sqref="A9:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -807,7 +806,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
@@ -818,7 +817,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B3" t="s">
@@ -829,7 +828,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
@@ -1021,7 +1020,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="2" t="s">
         <v>95</v>
       </c>
       <c r="B25" t="s">
@@ -1030,9 +1029,6 @@
       <c r="C25" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -1046,7 +1042,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B28" t="s">
@@ -1057,73 +1053,73 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="A29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>54</v>
       </c>
-      <c r="C29" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="C30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>55</v>
       </c>
-      <c r="C30" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="C31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" t="s">
         <v>48</v>
       </c>
-      <c r="C31" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="C32" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" t="s">
         <v>47</v>
       </c>
-      <c r="C32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+      <c r="C33" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>59</v>
       </c>
-      <c r="C33" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>82</v>
-      </c>
-      <c r="B34" t="s">
-        <v>81</v>
-      </c>
       <c r="C34" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="A35" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B35" t="s">
@@ -1133,39 +1129,28 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>45</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>62</v>
-      </c>
-      <c r="B39" t="s">
-        <v>64</v>
-      </c>
-      <c r="C39" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C40" t="s">
         <v>34</v>
@@ -1173,10 +1158,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C41" t="s">
         <v>34</v>
@@ -1184,12 +1169,23 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>68</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B43" t="s">
         <v>69</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C43" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>